<commit_message>
fix path names in binary files
</commit_message>
<xml_diff>
--- a/data/spreadsheets/Audio.xlsx
+++ b/data/spreadsheets/Audio.xlsx
@@ -5,18 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DDED3D-27F2-E040-A337-9A87B0A82D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507A476-F9C0-8B46-B743-7AF4F9832D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="67840" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -104,9 +115,6 @@
     <t>CC0 1.0</t>
   </si>
   <si>
-    <t>data/Multimedia_Data/Audio/</t>
-  </si>
-  <si>
     <t>Dramatis Personae</t>
   </si>
   <si>
@@ -485,6 +493,9 @@
   </si>
   <si>
     <t>AUD_throughthelookingglass_10.mp3</t>
+  </si>
+  <si>
+    <t>data/multimedia/audio/</t>
   </si>
 </sst>
 </file>
@@ -786,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -824,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -836,7 +847,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="116" customHeight="1">
@@ -844,10 +855,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
@@ -859,28 +870,28 @@
         <v>12</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="409.6">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -892,28 +903,28 @@
         <v>12</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="409.6">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -925,28 +936,28 @@
         <v>12</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="409.6">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -958,28 +969,28 @@
         <v>12</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="409.6">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
@@ -991,28 +1002,28 @@
         <v>12</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="409.6">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>10</v>
@@ -1024,28 +1035,28 @@
         <v>12</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="409.6">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
@@ -1057,28 +1068,28 @@
         <v>12</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="409.6">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>10</v>
@@ -1090,28 +1101,28 @@
         <v>12</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="409.6">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
@@ -1123,28 +1134,28 @@
         <v>12</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="409.6">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>10</v>
@@ -1156,28 +1167,28 @@
         <v>12</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="409.6">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>10</v>
@@ -1189,28 +1200,28 @@
         <v>12</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="409.6">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>10</v>
@@ -1222,28 +1233,28 @@
         <v>12</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="409.6">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
@@ -1255,64 +1266,64 @@
         <v>12</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="409.6">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="H15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="409.6">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>11</v>
@@ -1321,31 +1332,31 @@
         <v>12</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="409.6">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
@@ -1354,31 +1365,31 @@
         <v>12</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="409.6">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>11</v>
@@ -1387,31 +1398,31 @@
         <v>12</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="409.6">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>11</v>
@@ -1420,31 +1431,31 @@
         <v>12</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="409.6">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>11</v>
@@ -1453,31 +1464,31 @@
         <v>12</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="409.6">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>11</v>
@@ -1486,31 +1497,31 @@
         <v>12</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="409.6">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>11</v>
@@ -1519,31 +1530,31 @@
         <v>12</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="409.6">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>11</v>
@@ -1552,31 +1563,31 @@
         <v>12</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="409.6">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>11</v>
@@ -1585,32 +1596,32 @@
         <v>12</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="17" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="E25" s="1" t="s">
         <v>11</v>
       </c>
@@ -1618,16 +1629,16 @@
         <v>12</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I25" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" t="s">
         <v>89</v>
-      </c>
-      <c r="K25" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:11">

</xml_diff>

<commit_message>
test: set up automatic pytest runs (#20)
</commit_message>
<xml_diff>
--- a/data/spreadsheets/Audio.xlsx
+++ b/data/spreadsheets/Audio.xlsx
@@ -5,18 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DDED3D-27F2-E040-A337-9A87B0A82D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507A476-F9C0-8B46-B743-7AF4F9832D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="67840" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -104,9 +115,6 @@
     <t>CC0 1.0</t>
   </si>
   <si>
-    <t>data/Multimedia_Data/Audio/</t>
-  </si>
-  <si>
     <t>Dramatis Personae</t>
   </si>
   <si>
@@ -485,6 +493,9 @@
   </si>
   <si>
     <t>AUD_throughthelookingglass_10.mp3</t>
+  </si>
+  <si>
+    <t>data/multimedia/audio/</t>
   </si>
 </sst>
 </file>
@@ -786,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -824,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -836,7 +847,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="116" customHeight="1">
@@ -844,10 +855,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>10</v>
@@ -859,28 +870,28 @@
         <v>12</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="409.6">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
@@ -892,28 +903,28 @@
         <v>12</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="409.6">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>10</v>
@@ -925,28 +936,28 @@
         <v>12</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="409.6">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -958,28 +969,28 @@
         <v>12</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="409.6">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
@@ -991,28 +1002,28 @@
         <v>12</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="409.6">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>10</v>
@@ -1024,28 +1035,28 @@
         <v>12</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="409.6">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
@@ -1057,28 +1068,28 @@
         <v>12</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="409.6">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>10</v>
@@ -1090,28 +1101,28 @@
         <v>12</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="409.6">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>10</v>
@@ -1123,28 +1134,28 @@
         <v>12</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="409.6">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>10</v>
@@ -1156,28 +1167,28 @@
         <v>12</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="409.6">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>10</v>
@@ -1189,28 +1200,28 @@
         <v>12</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="409.6">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>10</v>
@@ -1222,28 +1233,28 @@
         <v>12</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="409.6">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>10</v>
@@ -1255,64 +1266,64 @@
         <v>12</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="409.6">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>87</v>
-      </c>
       <c r="H15" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="409.6">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>11</v>
@@ -1321,31 +1332,31 @@
         <v>12</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="409.6">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
@@ -1354,31 +1365,31 @@
         <v>12</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="409.6">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>11</v>
@@ -1387,31 +1398,31 @@
         <v>12</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="409.6">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>11</v>
@@ -1420,31 +1431,31 @@
         <v>12</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="409.6">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>11</v>
@@ -1453,31 +1464,31 @@
         <v>12</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="409.6">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>11</v>
@@ -1486,31 +1497,31 @@
         <v>12</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="409.6">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>11</v>
@@ -1519,31 +1530,31 @@
         <v>12</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="409.6">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>11</v>
@@ -1552,31 +1563,31 @@
         <v>12</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="409.6">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>11</v>
@@ -1585,32 +1596,32 @@
         <v>12</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="17" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="E25" s="1" t="s">
         <v>11</v>
       </c>
@@ -1618,16 +1629,16 @@
         <v>12</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>13</v>
+        <v>115</v>
       </c>
       <c r="I25" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="K25" t="s">
         <v>89</v>
-      </c>
-      <c r="K25" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:11">

</xml_diff>

<commit_message>
small correction on spreadsheet
</commit_message>
<xml_diff>
--- a/data/spreadsheets/Audio.xlsx
+++ b/data/spreadsheets/Audio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/daschland-scripts/data/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507A476-F9C0-8B46-B743-7AF4F9832D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E670B9A8-86D1-4847-B1E0-38CE61E2B51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20040" yWindow="1260" windowWidth="46200" windowHeight="30580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,9 +408,6 @@
 Shrill Voice/The Fishes: Liberty Stump</t>
   </si>
   <si>
-    <t>Lewis Carroll (Text), David Goldfarb (Book Coordinator, Editor), Elizabeth Klett (Meta Coordinator)</t>
-  </si>
-  <si>
     <t>Queen Alice, Shaking and Waking</t>
   </si>
   <si>
@@ -496,6 +493,9 @@
   </si>
   <si>
     <t>data/multimedia/audio/</t>
+  </si>
+  <si>
+    <t>Lewis Carroll (Text), David Goldfarb (Book Coordinator &amp; Editor), Elizabeth Klett (Meta Coordinator)</t>
   </si>
 </sst>
 </file>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -850,12 +850,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="116" customHeight="1">
+    <row r="2" spans="1:11" ht="409.6">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>73</v>
@@ -870,10 +870,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
@@ -888,7 +888,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>72</v>
@@ -903,10 +903,10 @@
         <v>12</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>15</v>
@@ -921,7 +921,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>71</v>
@@ -936,10 +936,10 @@
         <v>12</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>17</v>
@@ -954,7 +954,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>70</v>
@@ -969,10 +969,10 @@
         <v>12</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>19</v>
@@ -987,7 +987,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>69</v>
@@ -1002,10 +1002,10 @@
         <v>12</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>21</v>
@@ -1020,7 +1020,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>68</v>
@@ -1035,10 +1035,10 @@
         <v>12</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>23</v>
@@ -1053,7 +1053,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>67</v>
@@ -1068,10 +1068,10 @@
         <v>12</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>25</v>
@@ -1086,7 +1086,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>66</v>
@@ -1101,10 +1101,10 @@
         <v>12</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>27</v>
@@ -1119,7 +1119,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>65</v>
@@ -1134,10 +1134,10 @@
         <v>12</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>29</v>
@@ -1152,7 +1152,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>64</v>
@@ -1167,10 +1167,10 @@
         <v>12</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>31</v>
@@ -1185,7 +1185,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>63</v>
@@ -1200,10 +1200,10 @@
         <v>12</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>33</v>
@@ -1218,7 +1218,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>62</v>
@@ -1233,10 +1233,10 @@
         <v>12</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>35</v>
@@ -1251,7 +1251,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>61</v>
@@ -1266,10 +1266,10 @@
         <v>12</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>37</v>
@@ -1284,7 +1284,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>74</v>
@@ -1299,17 +1299,17 @@
         <v>12</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="409.6">
@@ -1317,7 +1317,7 @@
         <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>75</v>
@@ -1332,17 +1332,17 @@
         <v>12</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="409.6">
@@ -1350,7 +1350,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>76</v>
@@ -1368,14 +1368,14 @@
         <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>41</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="409.6">
@@ -1383,7 +1383,7 @@
         <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>77</v>
@@ -1401,14 +1401,14 @@
         <v>57</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="409.6">
@@ -1416,7 +1416,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>78</v>
@@ -1434,14 +1434,14 @@
         <v>57</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>45</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="409.6">
@@ -1449,7 +1449,7 @@
         <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>79</v>
@@ -1467,14 +1467,14 @@
         <v>57</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>47</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="409.6">
@@ -1482,7 +1482,7 @@
         <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>80</v>
@@ -1500,14 +1500,14 @@
         <v>57</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="409.6">
@@ -1515,7 +1515,7 @@
         <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>81</v>
@@ -1533,14 +1533,14 @@
         <v>57</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>51</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="409.6">
@@ -1548,7 +1548,7 @@
         <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>82</v>
@@ -1566,14 +1566,14 @@
         <v>57</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>53</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="409.6">
@@ -1581,7 +1581,7 @@
         <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>83</v>
@@ -1599,14 +1599,14 @@
         <v>57</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="17" customHeight="1">
@@ -1614,7 +1614,7 @@
         <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>84</v>
@@ -1632,13 +1632,13 @@
         <v>57</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K25" t="s">
         <v>88</v>
-      </c>
-      <c r="K25" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:11">

</xml_diff>

<commit_message>
small correction on spreadsheet (#31)
</commit_message>
<xml_diff>
--- a/data/spreadsheets/Audio.xlsx
+++ b/data/spreadsheets/Audio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/daschland-scripts/data/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507A476-F9C0-8B46-B743-7AF4F9832D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E670B9A8-86D1-4847-B1E0-38CE61E2B51D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20040" yWindow="1260" windowWidth="46200" windowHeight="30580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,9 +408,6 @@
 Shrill Voice/The Fishes: Liberty Stump</t>
   </si>
   <si>
-    <t>Lewis Carroll (Text), David Goldfarb (Book Coordinator, Editor), Elizabeth Klett (Meta Coordinator)</t>
-  </si>
-  <si>
     <t>Queen Alice, Shaking and Waking</t>
   </si>
   <si>
@@ -496,6 +493,9 @@
   </si>
   <si>
     <t>data/multimedia/audio/</t>
+  </si>
+  <si>
+    <t>Lewis Carroll (Text), David Goldfarb (Book Coordinator &amp; Editor), Elizabeth Klett (Meta Coordinator)</t>
   </si>
 </sst>
 </file>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -850,12 +850,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="116" customHeight="1">
+    <row r="2" spans="1:11" ht="409.6">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>73</v>
@@ -870,10 +870,10 @@
         <v>12</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
@@ -888,7 +888,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>72</v>
@@ -903,10 +903,10 @@
         <v>12</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>15</v>
@@ -921,7 +921,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>71</v>
@@ -936,10 +936,10 @@
         <v>12</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>17</v>
@@ -954,7 +954,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>70</v>
@@ -969,10 +969,10 @@
         <v>12</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>19</v>
@@ -987,7 +987,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>69</v>
@@ -1002,10 +1002,10 @@
         <v>12</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>21</v>
@@ -1020,7 +1020,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>68</v>
@@ -1035,10 +1035,10 @@
         <v>12</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>23</v>
@@ -1053,7 +1053,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>67</v>
@@ -1068,10 +1068,10 @@
         <v>12</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>25</v>
@@ -1086,7 +1086,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>66</v>
@@ -1101,10 +1101,10 @@
         <v>12</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>27</v>
@@ -1119,7 +1119,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>65</v>
@@ -1134,10 +1134,10 @@
         <v>12</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>29</v>
@@ -1152,7 +1152,7 @@
         <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>64</v>
@@ -1167,10 +1167,10 @@
         <v>12</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>31</v>
@@ -1185,7 +1185,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>63</v>
@@ -1200,10 +1200,10 @@
         <v>12</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>33</v>
@@ -1218,7 +1218,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>62</v>
@@ -1233,10 +1233,10 @@
         <v>12</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>35</v>
@@ -1251,7 +1251,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>61</v>
@@ -1266,10 +1266,10 @@
         <v>12</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>37</v>
@@ -1284,7 +1284,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>74</v>
@@ -1299,17 +1299,17 @@
         <v>12</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>13</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="409.6">
@@ -1317,7 +1317,7 @@
         <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>75</v>
@@ -1332,17 +1332,17 @@
         <v>12</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="409.6">
@@ -1350,7 +1350,7 @@
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>76</v>
@@ -1368,14 +1368,14 @@
         <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>41</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="409.6">
@@ -1383,7 +1383,7 @@
         <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>77</v>
@@ -1401,14 +1401,14 @@
         <v>57</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="409.6">
@@ -1416,7 +1416,7 @@
         <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>78</v>
@@ -1434,14 +1434,14 @@
         <v>57</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>45</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="409.6">
@@ -1449,7 +1449,7 @@
         <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>79</v>
@@ -1467,14 +1467,14 @@
         <v>57</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>47</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="409.6">
@@ -1482,7 +1482,7 @@
         <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>80</v>
@@ -1500,14 +1500,14 @@
         <v>57</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="409.6">
@@ -1515,7 +1515,7 @@
         <v>52</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>81</v>
@@ -1533,14 +1533,14 @@
         <v>57</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>51</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="409.6">
@@ -1548,7 +1548,7 @@
         <v>54</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>82</v>
@@ -1566,14 +1566,14 @@
         <v>57</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>53</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="409.6">
@@ -1581,7 +1581,7 @@
         <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>83</v>
@@ -1599,14 +1599,14 @@
         <v>57</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="17" customHeight="1">
@@ -1614,7 +1614,7 @@
         <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>84</v>
@@ -1632,13 +1632,13 @@
         <v>57</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I25" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K25" t="s">
         <v>88</v>
-      </c>
-      <c r="K25" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:11">

</xml_diff>